<commit_message>
feat: primeira versao funcionando, mas sem input pelas planilhas.
</commit_message>
<xml_diff>
--- a/financial_forecast_20241122.xlsx
+++ b/financial_forecast_20241122.xlsx
@@ -55,11 +55,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,391 +434,603 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="30" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Profit &amp; Loss Statement</t>
+          <t>Category</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Amount</t>
+          <t>Year 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Year 5</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Amount</t>
-        </is>
-      </c>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr"/>
+      <c r="C2" s="2" t="inlineStr"/>
+      <c r="D2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr"/>
+      <c r="F2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Revenue - - Product B</t>
+          <t>Product Sales</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>£55.00</t>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Revenue - - Product B</t>
+          <t>Service Revenue</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>£55.00</t>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Revenue - - Product A</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>£20.00</t>
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Total Revenue</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Revenue - - Product B</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>£50.00</t>
-        </is>
-      </c>
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Cost of Goods Sold (COGS)</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr"/>
+      <c r="C6" s="2" t="inlineStr"/>
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="inlineStr"/>
+      <c r="F6" s="2" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Revenue - - Total Revenue</t>
+          <t>Product Costs</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>£147.00</t>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Revenue - - Product A</t>
+          <t>Service Costs</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>£24.20</t>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Revenue - - Product B</t>
+          <t>IoT Device Costs</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>£60.50</t>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Revenue - - Product A</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>£20.00</t>
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Total COGS</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Revenue - - Product B</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>£50.00</t>
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Gross Profit</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Revenue - - Total Revenue</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>£154.70</t>
-        </is>
-      </c>
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>Operating Expenses</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr"/>
+      <c r="C12" s="2" t="inlineStr"/>
+      <c r="D12" s="2" t="inlineStr"/>
+      <c r="E12" s="2" t="inlineStr"/>
+      <c r="F12" s="2" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Revenue - - Product A</t>
+          <t>Marketing &amp; Sales</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>£26.62</t>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Revenue - - Product B</t>
+          <t>R&amp;D Expenses</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>£66.55</t>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Revenue - - Product A</t>
+          <t>Administrative Costs</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>£20.00</t>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Revenue - - Product B</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>£50.00</t>
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>Total Operating Expenses</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Revenue - - Total Revenue</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>£162.17</t>
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Operating Profit (EBIT)</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Revenue - - Product A</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>£29.28</t>
-        </is>
-      </c>
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Other Income/Expenses</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr"/>
+      <c r="C18" s="2" t="inlineStr"/>
+      <c r="D18" s="2" t="inlineStr"/>
+      <c r="E18" s="2" t="inlineStr"/>
+      <c r="F18" s="2" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Revenue - - Product B</t>
+          <t>Interest Expenses</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>£73.20</t>
+          <t>£5,000</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>£10,000</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>£10,000</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>£10,000</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>£10,000</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Revenue - - Product A</t>
+          <t>Tax (20%)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>£20.00</t>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>£0</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>£0</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Revenue - - Product B</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>£50.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Revenue - - Total Revenue</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>£172.48</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Revenue - - Product A</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>£32.21</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Revenue - - Product B</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>£80.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Total Revenue</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>£1,385.91</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Staff Costs</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>£1.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Services &amp; Software</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>£10,000.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Operating Expenses</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>£60,000.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Infrastructure &amp; Equipment</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>£1.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Other Expenses</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>£2,500.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Total Costs</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>£72,502.00</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Gross Profit</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>£-71,116.09</t>
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>Net Profit</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>£-5,000</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>£-10,000</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>£-10,000</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>£-10,000</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>£-10,000</t>
         </is>
       </c>
     </row>

</xml_diff>